<commit_message>
added yes with violations for monster combat 1 round
heheheh
</commit_message>
<xml_diff>
--- a/Iteration2-CorrectionGrid.xlsx
+++ b/Iteration2-CorrectionGrid.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="239">
   <si>
     <t>carrying capacity</t>
   </si>
@@ -871,6 +871,9 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>YES with violations</t>
   </si>
 </sst>
 </file>
@@ -1559,14 +1562,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A144" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A102" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.875" customWidth="1"/>
-    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2587,8 +2590,8 @@
       <c r="A110" t="s">
         <v>57</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>237</v>
+      <c r="B110" t="s">
+        <v>238</v>
       </c>
       <c r="C110" t="s">
         <v>126</v>

</xml_diff>